<commit_message>
Arrumando jupyter de recortes
</commit_message>
<xml_diff>
--- a/Recortes/final_db.xlsx
+++ b/Recortes/final_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrique Martinelli\redesoc-conteiner\notebooks\Projeto-RedesSoc\Recortes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D88A22F-486A-4E39-8EBF-48040D926ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F843AF70-1E84-4E22-A717-3AFDC30CB8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -868,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -878,6 +878,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1184,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AI10" sqref="AI10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,7 +1259,7 @@
       <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="W1" s="1" t="s">

</xml_diff>